<commit_message>
ultimos cambios abm Pedidos
</commit_message>
<xml_diff>
--- a/Control de funcionalidad.xlsx
+++ b/Control de funcionalidad.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>PRUEBAS</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Ver tema de Agregar un cartel "Administrar Pedidos" o "Administrar XXX " en los que no los tenga en Admin.aspx</t>
+  </si>
+  <si>
+    <t>Ver tema de quitar articulos de carrito luego de Confirmar un pedido</t>
   </si>
 </sst>
 </file>
@@ -438,73 +441,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -792,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:G18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,48 +809,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
       <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
@@ -862,67 +865,67 @@
       <c r="Y2" s="3"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="26" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="27" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
     </row>
     <row r="5" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="28" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
       <c r="R5" s="13" t="s">
         <v>18</v>
       </c>
@@ -937,25 +940,25 @@
       <c r="Y5" s="15"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="19" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="38"/>
       <c r="R6" s="10" t="s">
         <v>24</v>
       </c>
@@ -968,25 +971,25 @@
       <c r="Y6" s="12"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="19" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="38"/>
       <c r="R7" s="4"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
@@ -997,25 +1000,25 @@
       <c r="Y7" s="6"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="22" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="24"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="41"/>
       <c r="R8" s="10" t="s">
         <v>19</v>
       </c>
@@ -1028,15 +1031,15 @@
       <c r="Y8" s="12"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="42" t="s">
         <v>17</v>
       </c>
@@ -1057,25 +1060,25 @@
       <c r="Y9" s="6"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
       <c r="R10" s="10" t="s">
         <v>20</v>
       </c>
@@ -1088,25 +1091,25 @@
       <c r="Y10" s="12"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
       <c r="R11" s="4"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
@@ -1118,21 +1121,21 @@
       <c r="AC11" s="16"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
       <c r="R12" s="10" t="s">
         <v>22</v>
       </c>
@@ -1145,21 +1148,21 @@
       <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
       <c r="R13" s="4"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
@@ -1170,21 +1173,21 @@
       <c r="Y13" s="6"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
       <c r="R14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1197,21 +1200,21 @@
       <c r="Y14" s="12"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
       <c r="R15" s="4"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
@@ -1222,21 +1225,21 @@
       <c r="Y15" s="6"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
       <c r="R16" s="10" t="s">
         <v>25</v>
       </c>
@@ -1249,21 +1252,21 @@
       <c r="Y16" s="12"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
       <c r="R17" s="18"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
@@ -1274,21 +1277,21 @@
       <c r="Y17" s="6"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
       <c r="R18" s="10" t="s">
         <v>26</v>
       </c>
@@ -1301,21 +1304,21 @@
       <c r="Y18" s="12"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
       <c r="R19" s="4"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
@@ -1326,21 +1329,21 @@
       <c r="Y19" s="6"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
       <c r="R20" s="10" t="s">
         <v>31</v>
       </c>
@@ -1353,21 +1356,21 @@
       <c r="Y20" s="12"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
       <c r="R21" s="4"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
@@ -1378,21 +1381,21 @@
       <c r="Y21" s="6"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
       <c r="R22" s="10" t="s">
         <v>32</v>
       </c>
@@ -1405,21 +1408,21 @@
       <c r="Y22" s="12"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
       <c r="R23" s="4"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
@@ -1430,21 +1433,21 @@
       <c r="Y23" s="6"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
       <c r="R24" s="10" t="s">
         <v>35</v>
       </c>
@@ -1457,21 +1460,21 @@
       <c r="Y24" s="12"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
       <c r="R25" s="4"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
@@ -1482,46 +1485,48 @@
       <c r="Y25" s="6"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="6"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="R26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="12"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
       <c r="R27" s="4"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
@@ -1532,21 +1537,21 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
       <c r="R28" s="4"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
@@ -1557,21 +1562,21 @@
       <c r="Y28" s="6"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
       <c r="R29" s="4"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
@@ -1582,21 +1587,21 @@
       <c r="Y29" s="6"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
       <c r="R30" s="7"/>
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
@@ -1608,26 +1613,60 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="H11:O11"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="H2:O2"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="H8:O8"/>
+    <mergeCell ref="H9:O9"/>
+    <mergeCell ref="H10:O10"/>
+    <mergeCell ref="H23:O23"/>
+    <mergeCell ref="H12:O12"/>
+    <mergeCell ref="H13:O13"/>
+    <mergeCell ref="H14:O14"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="H16:O16"/>
+    <mergeCell ref="H17:O17"/>
+    <mergeCell ref="H18:O18"/>
+    <mergeCell ref="H19:O19"/>
+    <mergeCell ref="H20:O20"/>
+    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="H22:O22"/>
     <mergeCell ref="H30:O30"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
@@ -1644,60 +1683,26 @@
     <mergeCell ref="H27:O27"/>
     <mergeCell ref="H28:O28"/>
     <mergeCell ref="H29:O29"/>
-    <mergeCell ref="H23:O23"/>
-    <mergeCell ref="H12:O12"/>
-    <mergeCell ref="H13:O13"/>
-    <mergeCell ref="H14:O14"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="H16:O16"/>
-    <mergeCell ref="H17:O17"/>
-    <mergeCell ref="H18:O18"/>
-    <mergeCell ref="H19:O19"/>
-    <mergeCell ref="H20:O20"/>
-    <mergeCell ref="H21:O21"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="H11:O11"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="H2:O2"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="H7:O7"/>
-    <mergeCell ref="H8:O8"/>
-    <mergeCell ref="H9:O9"/>
-    <mergeCell ref="H10:O10"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>